<commit_message>
Update Mappings 22 Ontologies
</commit_message>
<xml_diff>
--- a/MappingHeatmap.xlsx
+++ b/MappingHeatmap.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
   <si>
     <t>AFO</t>
   </si>
@@ -31,16 +31,28 @@
     <t>ChEBI</t>
   </si>
   <si>
+    <t>CHEMINF</t>
+  </si>
+  <si>
     <t>CHMO</t>
   </si>
   <si>
+    <t>CIF</t>
+  </si>
+  <si>
     <t>EDAM</t>
   </si>
   <si>
+    <t>EMMO</t>
+  </si>
+  <si>
     <t>ENVO</t>
   </si>
   <si>
-    <t>metadata4Ing</t>
+    <t>M3</t>
+  </si>
+  <si>
+    <t>metadata4ing</t>
   </si>
   <si>
     <t>MOP</t>
@@ -52,13 +64,10 @@
     <t>OBI</t>
   </si>
   <si>
-    <t>OFM</t>
+    <t>OM</t>
   </si>
   <si>
     <t>OSMO</t>
-  </si>
-  <si>
-    <t>PIMS-II</t>
   </si>
   <si>
     <t>REX</t>
@@ -428,13 +437,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:W23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:23">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -492,21 +501,30 @@
       <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:20">
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:23">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -517,7 +535,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:23">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -525,13 +543,13 @@
         <v>121</v>
       </c>
       <c r="C5">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:23">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -539,7 +557,7 @@
         <v>58</v>
       </c>
       <c r="C6">
-        <v>1489</v>
+        <v>1678</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -548,556 +566,751 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:23">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>249</v>
+        <v>92</v>
       </c>
       <c r="C7">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="D7">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="E7">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="F7">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>50</v>
+        <v>249</v>
       </c>
       <c r="C8">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E8">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="F8">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="G8">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>207</v>
+        <v>128</v>
       </c>
       <c r="C9">
-        <v>192</v>
+        <v>24</v>
       </c>
       <c r="D9">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="E9">
-        <v>78</v>
+        <v>19</v>
       </c>
       <c r="F9">
-        <v>938</v>
+        <v>12</v>
       </c>
       <c r="G9">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="H9">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G10">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="I10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>6</v>
+        <v>144</v>
       </c>
       <c r="C11">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E11">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F11">
-        <v>58</v>
+        <v>23</v>
       </c>
       <c r="G11">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I11">
-        <v>25</v>
+        <v>502</v>
       </c>
       <c r="J11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>139</v>
+        <v>248</v>
       </c>
       <c r="C12">
-        <v>45</v>
+        <v>212</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="E12">
-        <v>26</v>
+        <v>84</v>
       </c>
       <c r="F12">
-        <v>20</v>
+        <v>939</v>
       </c>
       <c r="G12">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="H12">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="I12">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="J12">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="K12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>204</v>
+        <v>88</v>
       </c>
       <c r="C13">
-        <v>152</v>
+        <v>27</v>
       </c>
       <c r="D13">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>73</v>
+        <v>19</v>
       </c>
       <c r="F13">
-        <v>129</v>
+        <v>9</v>
       </c>
       <c r="G13">
-        <v>78</v>
+        <v>8</v>
       </c>
       <c r="H13">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="I13">
-        <v>182</v>
+        <v>67</v>
       </c>
       <c r="J13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K13">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="L13">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C14">
         <v>2</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E14">
+        <v>7</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
         <v>4</v>
       </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>2</v>
-      </c>
       <c r="H14">
         <v>3</v>
       </c>
       <c r="I14">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="J14">
         <v>1</v>
       </c>
       <c r="K14">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M14">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B15">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>7</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="E15">
         <v>8</v>
       </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>2</v>
-      </c>
       <c r="F15">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I15">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K15">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L15">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="M15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B16">
-        <v>21</v>
+        <v>140</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G16">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="H16">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="I16">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="J16">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="K16">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="L16">
-        <v>1</v>
+        <v>75</v>
       </c>
       <c r="M16">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="N16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>9</v>
+        <v>289</v>
       </c>
       <c r="C17">
-        <v>7</v>
+        <v>172</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="E17">
-        <v>2</v>
+        <v>82</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>136</v>
       </c>
       <c r="G17">
-        <v>18</v>
+        <v>236</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="I17">
+        <v>61</v>
+      </c>
+      <c r="J17">
+        <v>48</v>
+      </c>
+      <c r="K17">
+        <v>54</v>
+      </c>
+      <c r="L17">
+        <v>399</v>
+      </c>
+      <c r="M17">
+        <v>97</v>
+      </c>
+      <c r="N17">
         <v>6</v>
       </c>
-      <c r="J17">
-        <v>1</v>
-      </c>
-      <c r="K17">
-        <v>23</v>
-      </c>
-      <c r="L17">
-        <v>2</v>
-      </c>
-      <c r="M17">
-        <v>3</v>
-      </c>
-      <c r="N17">
-        <v>0</v>
-      </c>
       <c r="O17">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="P17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>14</v>
+        <v>100</v>
       </c>
       <c r="C18">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E18">
         <v>17</v>
       </c>
       <c r="F18">
-        <v>228</v>
+        <v>11</v>
       </c>
       <c r="G18">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I18">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="J18">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K18">
-        <v>122</v>
+        <v>78</v>
       </c>
       <c r="L18">
-        <v>3</v>
+        <v>226</v>
       </c>
       <c r="M18">
-        <v>12</v>
+        <v>131</v>
       </c>
       <c r="N18">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O18">
         <v>0</v>
       </c>
       <c r="P18">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="Q18">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B19">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="C19">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
         <v>2</v>
       </c>
-      <c r="E19">
-        <v>7</v>
-      </c>
       <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>8</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>5</v>
+      </c>
+      <c r="J19">
+        <v>4</v>
+      </c>
+      <c r="K19">
+        <v>4</v>
+      </c>
+      <c r="L19">
         <v>13</v>
       </c>
-      <c r="G19">
-        <v>3</v>
-      </c>
-      <c r="H19">
-        <v>7</v>
-      </c>
-      <c r="I19">
-        <v>16</v>
-      </c>
-      <c r="J19">
-        <v>1</v>
-      </c>
-      <c r="K19">
+      <c r="M19">
+        <v>4</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>3</v>
+      </c>
+      <c r="Q19">
         <v>19</v>
       </c>
-      <c r="L19">
-        <v>9</v>
-      </c>
-      <c r="M19">
-        <v>13</v>
-      </c>
-      <c r="N19">
-        <v>3</v>
-      </c>
-      <c r="O19">
-        <v>1</v>
-      </c>
-      <c r="P19">
-        <v>2</v>
-      </c>
-      <c r="Q19">
-        <v>11</v>
-      </c>
       <c r="R19">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B20">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>7</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>18</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>16</v>
+      </c>
+      <c r="M20">
+        <v>6</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <v>23</v>
+      </c>
+      <c r="P20">
+        <v>2</v>
+      </c>
+      <c r="Q20">
+        <v>7</v>
+      </c>
+      <c r="R20">
+        <v>1</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22">
+      <c r="A21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>14</v>
+      </c>
+      <c r="C21">
+        <v>8</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <v>17</v>
+      </c>
+      <c r="F21">
+        <v>230</v>
+      </c>
+      <c r="G21">
+        <v>5</v>
+      </c>
+      <c r="H21">
+        <v>10</v>
+      </c>
+      <c r="I21">
+        <v>5</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>4</v>
+      </c>
+      <c r="L21">
+        <v>95</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+      <c r="O21">
+        <v>123</v>
+      </c>
+      <c r="P21">
+        <v>3</v>
+      </c>
+      <c r="Q21">
+        <v>16</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22">
+      <c r="A22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>41</v>
+      </c>
+      <c r="C22">
+        <v>27</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>7</v>
+      </c>
+      <c r="F22">
+        <v>13</v>
+      </c>
+      <c r="G22">
+        <v>9</v>
+      </c>
+      <c r="H22">
+        <v>3</v>
+      </c>
+      <c r="I22">
+        <v>14</v>
+      </c>
+      <c r="J22">
+        <v>7</v>
+      </c>
+      <c r="K22">
+        <v>17</v>
+      </c>
+      <c r="L22">
+        <v>62</v>
+      </c>
+      <c r="M22">
+        <v>11</v>
+      </c>
+      <c r="N22">
+        <v>1</v>
+      </c>
+      <c r="O22">
+        <v>20</v>
+      </c>
+      <c r="P22">
+        <v>9</v>
+      </c>
+      <c r="Q22">
+        <v>31</v>
+      </c>
+      <c r="R22">
+        <v>31</v>
+      </c>
+      <c r="S22">
+        <v>1</v>
+      </c>
+      <c r="T22">
+        <v>11</v>
+      </c>
+      <c r="U22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22">
+      <c r="A23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23">
         <v>83</v>
       </c>
-      <c r="C20">
+      <c r="C23">
+        <v>13</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <v>19</v>
+      </c>
+      <c r="F23">
+        <v>3</v>
+      </c>
+      <c r="G23">
+        <v>33</v>
+      </c>
+      <c r="H23">
+        <v>5</v>
+      </c>
+      <c r="I23">
+        <v>83</v>
+      </c>
+      <c r="J23">
+        <v>15</v>
+      </c>
+      <c r="K23">
+        <v>90</v>
+      </c>
+      <c r="L23">
+        <v>74</v>
+      </c>
+      <c r="M23">
+        <v>37</v>
+      </c>
+      <c r="N23">
+        <v>8</v>
+      </c>
+      <c r="O23">
+        <v>1</v>
+      </c>
+      <c r="P23">
         <v>12</v>
       </c>
-      <c r="D20">
-        <v>3</v>
-      </c>
-      <c r="E20">
-        <v>19</v>
-      </c>
-      <c r="F20">
-        <v>3</v>
-      </c>
-      <c r="G20">
-        <v>5</v>
-      </c>
-      <c r="H20">
-        <v>15</v>
-      </c>
-      <c r="I20">
-        <v>21</v>
-      </c>
-      <c r="J20">
-        <v>6</v>
-      </c>
-      <c r="K20">
-        <v>1</v>
-      </c>
-      <c r="L20">
-        <v>12</v>
-      </c>
-      <c r="M20">
-        <v>24</v>
-      </c>
-      <c r="N20">
-        <v>8</v>
-      </c>
-      <c r="O20">
+      <c r="Q23">
+        <v>96</v>
+      </c>
+      <c r="R23">
+        <v>72</v>
+      </c>
+      <c r="S23">
         <v>172</v>
       </c>
-      <c r="P20">
-        <v>18</v>
-      </c>
-      <c r="Q20">
-        <v>0</v>
-      </c>
-      <c r="R20">
+      <c r="T23">
+        <v>0</v>
+      </c>
+      <c r="U23">
         <v>2</v>
       </c>
-      <c r="S20">
+      <c r="V23">
         <v>9</v>
       </c>
     </row>

</xml_diff>